<commit_message>
Page Factory MS Error Fix
</commit_message>
<xml_diff>
--- a/Page Factory/POM1/POM1/DataAccess/TestData.xlsx
+++ b/Page Factory/POM1/POM1/DataAccess/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Selenium\NUnit Testing\Page Factory\POM1\POM1\DataAccess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4E22C8-6252-4A47-BC20-AF1E2EA6C29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840356D3-3A22-4E82-BAE7-CE79C696EA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE03AD66-2DC1-473A-831F-798BB6754AFC}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>